<commit_message>
preping for CD36 alignment
</commit_message>
<xml_diff>
--- a/gene_list_spreadsheet.xlsx
+++ b/gene_list_spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackcross/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackcross/Documents/meat_vs_fat_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E6A2F3B-115D-D74B-B4EA-93B4AF447170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E451CA6-882F-8943-AEF8-385D20A6F33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{D36F015F-F9CE-2C47-849E-CCFCE8EA282F}"/>
+    <workbookView xWindow="-30340" yWindow="3840" windowWidth="28040" windowHeight="17440" xr2:uid="{D36F015F-F9CE-2C47-849E-CCFCE8EA282F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Function</t>
   </si>
@@ -60,6 +59,15 @@
   </si>
   <si>
     <t xml:space="preserve">Binds short chain saturated fatty acids </t>
+  </si>
+  <si>
+    <t>CD36</t>
+  </si>
+  <si>
+    <t>long-chain fatty acid and lipoprotein presception</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/hmg/article/17/11/1695/599714</t>
   </si>
 </sst>
 </file>
@@ -420,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A547AE-F186-9541-96FE-1247DA02C4CB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -465,6 +473,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>